<commit_message>
Renovation: Updated, Sankey: AMPLpy + color
</commit_message>
<xml_diff>
--- a/ColorSankey.xlsx
+++ b/ColorSankey.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/achuat/Documents/Projects/Governance_EnergyScope/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/achuat/Documents/Projects/Governance_EnergyScope/EnergyScopePy_dev/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03DD6006-F329-F046-96BE-85559B5FB30A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48786808-54A4-734D-8C73-0AE78647DA35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -218,7 +218,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -349,6 +349,13 @@
     <font>
       <sz val="12"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -695,8 +702,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1055,7 +1063,7 @@
   <dimension ref="A1:C58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1065,11 +1073,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" t="s">
         <v>34</v>
-      </c>
-      <c r="B1" t="s">
-        <v>35</v>
       </c>
       <c r="C1" t="s">
         <v>36</v>

</xml_diff>